<commit_message>
modified exp2ipynb folder for local module load
</commit_message>
<xml_diff>
--- a/Article/2010_ExpressionAnalysisCompare.xlsx
+++ b/Article/2010_ExpressionAnalysisCompare.xlsx
@@ -10,7 +10,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="RFClassComp" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="RFRegrComp" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="82">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -268,33 +267,6 @@
   </si>
   <si>
     <t xml:space="preserve">0.18, 0.11, 0.08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mutalik et al. (2010)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geobac.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2 CV Mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2 CV Std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2 Train</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2 Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-28:A,-33:T,-20:A]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.16, 0.09, 0.08</t>
   </si>
 </sst>
 </file>
@@ -410,11 +382,11 @@
   </sheetPr>
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.02"/>
@@ -1469,10 +1441,10 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
@@ -2259,377 +2231,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J18"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.88"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="n">
-        <v>1232</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="n">
-        <v>9684</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="n">
-        <v>1080</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="n">
-        <v>289</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="n">
-        <f aca="false">0.16+0.09+0.08</f>
-        <v>0.33</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>